<commit_message>
programa mesas casi terminado
</commit_message>
<xml_diff>
--- a/Congreso_2018/Copia de Programación Mesas Temáticas FINAL.xlsx
+++ b/Congreso_2018/Copia de Programación Mesas Temáticas FINAL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Miércoles" sheetId="1" state="visible" r:id="rId2"/>
@@ -5197,9 +5197,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>875520</xdr:colOff>
+      <xdr:colOff>874800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5213,7 +5213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="875520" cy="8181720"/>
+          <a:ext cx="874800" cy="8181000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5239,9 +5239,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1630800</xdr:rowOff>
+      <xdr:rowOff>1630440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5255,7 +5255,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="656640" cy="13395240"/>
+          <a:ext cx="655920" cy="13394880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5281,9 +5281,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>913680</xdr:colOff>
+      <xdr:colOff>912960</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5297,7 +5297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="913680" cy="13745520"/>
+          <a:ext cx="912960" cy="13744800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5319,8 +5319,8 @@
   </sheetPr>
   <dimension ref="B1:P4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5528,8 +5528,8 @@
   </sheetPr>
   <dimension ref="B1:R9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5970,7 +5970,7 @@
   <dimension ref="B1:Q9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>